<commit_message>
survey response appendix and writeup updated
</commit_message>
<xml_diff>
--- a/doc/FinalSubmission/Survey Responses.xlsx
+++ b/doc/FinalSubmission/Survey Responses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Documents\GitHub\augreality\doc\FinalSubmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Comfort</t>
   </si>
@@ -45,14 +45,34 @@
   </si>
   <si>
     <t>Framerate</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,48 +383,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B1" sqref="B1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>5</v>
       </c>
@@ -414,105 +432,141 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <v>4</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:H7" si="0">AVERAGE(C2:C6)</f>
+        <v>3.8</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>